<commit_message>
MetaEd v1.4.1 Output run against v3.0 DS and ODS/API
</commit_message>
<xml_diff>
--- a/DelawareExtensionProject/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
+++ b/DelawareExtensionProject/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
@@ -423,16 +423,16 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>247</v>
+        <v>595</v>
       </c>
       <c r="B2" t="str">
-        <v>TitleIPartAParticipant</v>
+        <v>EducationOrganizationInterventionPrescriptionAssociation</v>
       </c>
       <c r="C2" t="str">
-        <v>An indication of the type of Title I program, if any, in which the student is participating and served.</v>
+        <v>This association indicates interventions made available by an education organization. Often, a district-level education organization purchases a set of intervention prescriptions and makes them available to its schools for use on demand.</v>
       </c>
       <c r="D2" t="str">
-        <v>Descriptor</v>
+        <v>Association</v>
       </c>
       <c r="E2" t="str">
         <v/>
@@ -441,57 +441,13 @@
         <v/>
       </c>
       <c r="G2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Used By:
-StudentTitleIPartAProgramAssociation.TitleIPartAParticipant (as required)</v>
-      </c>
-      <c r="H2" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;xs:complexType name="TitleIPartAParticipantDescriptor"&gt;
-  &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;An indication of the type of Title I program, if any, in which the student is participating and served.&lt;/xs:documentation&gt;
-    &lt;xs:appinfo&gt;
-      &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
-    &lt;/xs:appinfo&gt;
-  &lt;/xs:annotation&gt;
-  &lt;xs:complexContent&gt;
-    &lt;xs:extension base="DescriptorType" /&gt;
-  &lt;/xs:complexContent&gt;
-&lt;/xs:complexType&gt;</v>
-      </c>
-      <c r="I2" t="str" xml:space="preserve">
-        <v xml:space="preserve">edfi.TitleIPartAParticipantDescriptor
-TitleIPartAParticipantDescriptorId [INT] NOT NULL
-Primary Keys:
-TitleIPartAParticipantDescriptorId
-</v>
-      </c>
-    </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>595</v>
-      </c>
-      <c r="B3" t="str">
-        <v>EducationOrganizationInterventionPrescriptionAssociation</v>
-      </c>
-      <c r="C3" t="str">
-        <v>This association indicates interventions made available by an education organization. Often, a district-level education organization purchases a set of intervention prescriptions and makes them available to its schools for use on demand.</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Association</v>
-      </c>
-      <c r="E3" t="str">
-        <v/>
-      </c>
-      <c r="F3" t="str">
-        <v/>
-      </c>
-      <c r="G3" t="str" xml:space="preserve">
         <v xml:space="preserve">Contains:
 BeginDate (optional)
 EducationOrganization (identity)
 EndDate (optional)
 InterventionPrescription (identity)</v>
       </c>
-      <c r="H3" t="str" xml:space="preserve">
+      <c r="H2" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="EducationOrganizationInterventionPrescriptionAssociation"&gt;
   &lt;xs:annotation&gt;
     &lt;xs:documentation&gt;This association indicates interventions made available by an education organization. Often, a district-level education organization purchases a set of intervention prescriptions and makes them available to its schools for use on demand.&lt;/xs:documentation&gt;
@@ -527,7 +483,7 @@
   &lt;/xs:complexContent&gt;
 &lt;/xs:complexType&gt;</v>
       </c>
-      <c r="I3" t="str" xml:space="preserve">
+      <c r="I2" t="str" xml:space="preserve">
         <v xml:space="preserve">edfi.EducationOrganizationInterventionPrescriptionAssociation
 EducationOrganizationId [INT] NOT NULL
 InterventionPrescriptionEducationOrganizationId [INT] NOT NULL
@@ -541,6 +497,83 @@
 EducationOrganizationId
 InterventionPrescriptionEducationOrganizationId
 InterventionPrescriptionIdentificationCode
+</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>596</v>
+      </c>
+      <c r="B3" t="str">
+        <v>EducationOrganizationNetworkAssociation</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Properties of the association between the EducationOrganization and its network(s).</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Association</v>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str" xml:space="preserve">
+        <v xml:space="preserve">Contains:
+BeginDate (optional)
+EducationOrganization (identity)
+EducationOrganizationNetwork (identity)
+EndDate (optional)</v>
+      </c>
+      <c r="H3" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;xs:complexType name="EducationOrganizationNetworkAssociation"&gt;
+  &lt;xs:annotation&gt;
+    &lt;xs:documentation&gt;Properties of the association between the EducationOrganization and its network(s).&lt;/xs:documentation&gt;
+    &lt;xs:appinfo&gt;
+      &lt;ann:TypeGroup&gt;Association&lt;/ann:TypeGroup&gt;
+    &lt;/xs:appinfo&gt;
+  &lt;/xs:annotation&gt;
+  &lt;xs:complexContent&gt;
+    &lt;xs:extension base="ComplexObjectType"&gt;
+      &lt;xs:sequence&gt;
+        &lt;xs:element name="EducationOrganizationNetworkReference" type="EducationOrganizationNetworkReferenceType"&gt;
+          &lt;xs:annotation&gt;
+            &lt;xs:documentation&gt;A reference to the EducationOrganizationNetwork to which this education organization is a member.&lt;/xs:documentation&gt;
+          &lt;/xs:annotation&gt;
+        &lt;/xs:element&gt;
+        &lt;xs:element name="MemberEducationOrganizationReference" type="EducationOrganizationReferenceType"&gt;
+          &lt;xs:annotation&gt;
+            &lt;xs:documentation&gt;The EducationOrganization member in the network.&lt;/xs:documentation&gt;
+          &lt;/xs:annotation&gt;
+        &lt;/xs:element&gt;
+        &lt;xs:element name="BeginDate" type="xs:date" minOccurs="0"&gt;
+          &lt;xs:annotation&gt;
+            &lt;xs:documentation&gt;The date on which the EducationOrganization joined this network.&lt;/xs:documentation&gt;
+          &lt;/xs:annotation&gt;
+        &lt;/xs:element&gt;
+        &lt;xs:element name="EndDate" type="xs:date" minOccurs="0"&gt;
+          &lt;xs:annotation&gt;
+            &lt;xs:documentation&gt;The date on which the EducationOrganization left this network.&lt;/xs:documentation&gt;
+          &lt;/xs:annotation&gt;
+        &lt;/xs:element&gt;
+      &lt;/xs:sequence&gt;
+    &lt;/xs:extension&gt;
+  &lt;/xs:complexContent&gt;
+&lt;/xs:complexType&gt;</v>
+      </c>
+      <c r="I3" t="str" xml:space="preserve">
+        <v xml:space="preserve">edfi.EducationOrganizationNetworkAssociation
+EducationOrganizationNetworkId [INT] NOT NULL
+MemberEducationOrganizationId [INT] NOT NULL
+BeginDate [DATE] NULL
+EndDate [DATE] NULL
+CreateDate [DATETIME] NOT NULL
+LastModifiedDate [DATETIME] NOT NULL
+Id [UNIQUEIDENTIFIER] NOT NULL
+Primary Keys:
+EducationOrganizationNetworkId
+MemberEducationOrganizationId
 </v>
       </c>
     </row>
@@ -1193,8 +1226,7 @@
       <c r="H10" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="StaffEducationOrganizationEmploymentAssociation"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This association indicates the EducationOrganization an employee, contractor, volunteer, or other service provider is formally associated with typically indicated by which organization the staff member has a services contract with or receives compensation
-      from.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This association indicates the EducationOrganization an employee, contractor, volunteer, or other service provider is formally associated with typically indicated by which organization the staff member has a services contract with or receives compensation from.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Association&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -1214,8 +1246,13 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="EmploymentStatus" type="EmploymentStatusDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Reflects the type of employment or contract; for example: Probationary Contractual Substitute/temporary Tenured or permanent Volunteer/no contract ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Reflects the type of employment or contract; for example:
+              Probationary
+              Contractual
+              Substitute/temporary
+              Tenured or permanent
+              Volunteer/no contract
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;EmploymentStatusDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -1428,7 +1465,12 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="ProgramAssignment" type="ProgramAssignmentDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The name of the program for which the individual is assigned; for example: Regular education Title I-Academic Title I-Non-Academic Special Education Bilingual/English as a Second Language.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The name of the program for which the individual is assigned; for example:
+              Regular education
+              Title I-Academic
+              Title I-Non-Academic
+              Special Education
+              Bilingual/English as a Second Language.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;ProgramAssignmentDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -1552,7 +1594,8 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="ClassroomPosition" type="ClassroomPositionDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The type of position the Staff member holds in the specific class/section; for example: Teacher of Record, Assistant Teacher, Support Teacher, Substitute Teacher...&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The type of position the Staff member holds in the specific class/section; for example:
+              Teacher of Record, Assistant Teacher, Support Teacher, Substitute Teacher...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;ClassroomPositionDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -1580,8 +1623,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="PercentageContribution" type="Percent" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Indicates the percentage of the total scheduled course time, academic standards, and/or learning activities delivered in this section by this staff member. A teacher of record designation may be based solely or partially on this contribution
-              percentage.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Indicates the percentage of the total scheduled course time, academic standards, and/or learning activities delivered in this section by this staff member. A teacher of record designation may be based solely or partially on this contribution percentage.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
       &lt;/xs:sequence&gt;
@@ -1774,8 +1816,12 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="StudentParticipationCode" type="StudentParticipationCodeDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The role or type of participation of a student in a discipline incident; for example: Victim Perpetrator Witness Reporter.
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The role or type of participation of a student in a discipline incident;
+              for example:
+              Victim
+              Perpetrator
+              Witness
+              Reporter.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;StudentParticipationCodeDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -1923,13 +1969,17 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="HispanicLatinoEthnicity" type="xs:boolean" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;An indication that the individual traces his or her origin or descent to Mexico, Puerto Rico, Cuba, Central, and South America, and other Spanish cultures, regardless of race. The term, "Spanish origin," can be used in addition to "Hispanic
-              or Latino."&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;An indication that the individual traces his or her origin or descent to Mexico, Puerto Rico, Cuba, Central, and South America, and other Spanish cultures, regardless of race. The term, "Spanish origin," can be used in addition to "Hispanic or Latino."&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="OldEthnicity" type="OldEthnicityDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Previous definition of Ethnicity combining Hispanic/Latino and race: 1 - American Indian or Alaskan Native 2 - Asian or Pacific Islander 3 - Black, not of Hispanic origin 4 - Hispanic 5 - White, not of Hispanic origin.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Previous definition of Ethnicity combining Hispanic/Latino and race:
+              1 - American Indian or Alaskan Native
+              2 - Asian or Pacific Islander
+              3 - Black, not of Hispanic origin
+              4 - Hispanic
+              5 - White, not of Hispanic origin.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;OldEthnicityDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -1937,8 +1987,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="Race" type="RaceDescriptorReferenceType" minOccurs="0" maxOccurs="unbounded"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The general racial category which most clearly reflects the individual's recognition of his or her community or with which the individual most identifies. The data model allows for multiple entries so that each individual can specify all appropriate
-              races.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The general racial category which most clearly reflects the individual's recognition of his or her community or with which the individual most identifies. The data model allows for multiple entries so that each individual can specify all appropriate races.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;RaceDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -1954,7 +2003,8 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="StudentCharacteristic" type="StudentCharacteristic" minOccurs="0" maxOccurs="unbounded"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Reflects important characteristics of the student's home situation: Displaced Homemaker, Immigrant, Migratory, Military Parent, Pregnant Teen, Single Parent, and Unaccompanied Youth.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Reflects important characteristics of the student's home situation:
+              Displaced Homemaker, Immigrant, Migratory, Military Parent, Pregnant Teen, Single Parent, and Unaccompanied Youth.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="LimitedEnglishProficiency" type="LimitedEnglishProficiencyDescriptorReferenceType" minOccurs="0"&gt;
@@ -2392,8 +2442,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="InterventionEffectiveness" type="InterventionEffectiveness" minOccurs="0" maxOccurs="unbounded"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;A measure of the effects of an intervention in each outcome domain. The rating of effectiveness takes into account four factors: the quality of the research on the intervention, the statistical significance of the research findings, the size
-              of the differences between participants in the intervention and comparison groups and the consistency in results.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;A measure of the effects of an intervention in each outcome domain. The rating of effectiveness takes into account four factors: the quality of the research on the intervention, the statistical significance of the research findings, the size of the differences between participants in the intervention and comparison groups and the consistency in results.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="DiagnosticStatement" type="DiagnosticStatement" minOccurs="0"&gt;
@@ -2500,7 +2549,8 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="Relation" type="RelationDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The nature of an individual's relationship to a student; for example: Father, Mother, Step Father, Step Mother, Foster Father, Foster Mother, Guardian, etc.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The nature of an individual's relationship to a student; for example:
+              Father, Mother, Step Father, Step Mother, Foster Father, Foster Mother, Guardian, etc.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;RelationDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -2834,8 +2884,11 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="RepeatIdentifier" type="RepeatIdentifierDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;An indication as to whether a student has previously taken a given course. Repeated, counted in grade point average Repeated, not counted in grade point average Not repeated Other.
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;An indication as to whether a student has previously taken a given course.
+              Repeated, counted in grade point average
+              Repeated, not counted in grade point average
+              Not repeated
+              Other.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;RepeatIdentifierDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -2942,8 +2995,8 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="PrivateCTEProgram" type="xs:boolean" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Indicator that student participated in career and technical education at private agencies or institutions that are reported by the state for purposes of the Elementary and Secondary Education Act (ESEA). Students in private institutions which
-              do not receive Perkins funding are reported only in the state file.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Indicator that student participated in career and technical education at private agencies or institutions that are reported by the state for purposes of the Elementary and Secondary Education Act (ESEA).
+              Students in private institutions which do not receive Perkins funding are reported only in the state file.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="TechnicalSkillsAssessment" type="TechnicalSkillsAssessmentDescriptorReferenceType" minOccurs="0"&gt;
@@ -3072,8 +3125,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="HomelessUnaccompaniedYouth" type="xs:boolean" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;A homeless unaccompanied youth is a youth who is not in the physical custody of a parent or guardian and who fits the McKinney-Vento definition of homeless. Students must be both unaccompanied and homeless to be included as an unaccompanied
-              homeless youth.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;A homeless unaccompanied youth is a youth who is not in the physical custody of a parent or guardian and who fits the McKinney-Vento definition of homeless. Students must be both unaccompanied and homeless to be included as an unaccompanied homeless youth.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="HomelessProgramService" type="HomelessProgramService" minOccurs="0" maxOccurs="unbounded"&gt;
@@ -3288,8 +3340,7 @@
       &lt;xs:sequence&gt;
         &lt;xs:element name="PriorityForServices" type="xs:boolean"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Report migratory children who are classified as having "priority for services" because they are failing, or most at risk of failing to meet the State's challenging State academic content standards and challenging State student academic achievement
-              standards, and their education has been interrupted during the regular school year.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Report migratory children who are classified as having "priority for services" because they are failing, or most at risk of failing to meet the State's challenging State academic content standards and challenging State student academic achievement standards, and their education has been interrupted during the regular school year.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="LastQualifyingMove" type="xs:date"&gt;
@@ -3299,9 +3350,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="ContinuationOfServicesReason" type="ContinuationOfServicesReasonDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The "continuation of services" provision found in Section 1304(e) of the statute provides that (1) a child who ceases to be a migratory child during a school term shall be eligible for services until the end of such term; (2) a child who is
-              no longer a migratory child may continue to receive services for one additional school year, but only if comparable services are not available through other programs; and (3) secondary school students who were eligible for services in secondary
-              school may continue to be served through credit accrual programs until graduation. Only students who received services at any time during their 36 month eligibility period may continue to receive services (not necessarily the same service).&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The "continuation of services" provision found in Section 1304(e) of the statute provides that (1) a child who ceases to be a migratory child during a school term shall be eligible for services until the end of such term; (2) a child who is no longer a migratory child may continue to receive services for one additional school year, but only if comparable services are not available through other programs; and (3) secondary school students who were eligible for services in secondary school may continue to be served through credit accrual programs until graduation. Only students who received services at any time during their 36 month eligibility period may continue to receive services (not necessarily the same service).&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;ContinuationOfServicesReasonDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -3324,8 +3373,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="QualifyingArrivalDate" type="xs:date" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The Qualifying Arrival Date (QAD) is the date the child joins the worker who has already moved, or the date when the worker joins the child who has already moved. The QAD is the date that the child’s eligibility for the MEP begins. The QAD
-              is not affected by subsequent non-qualifying moves.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The Qualifying Arrival Date (QAD) is the date the child joins the worker who has already moved, or the date when the worker joins the child who has already moved. The QAD is the date that the child’s eligibility for the MEP begins. The QAD is not affected by subsequent non-qualifying moves.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="StateResidencyDate" type="xs:date" minOccurs="0"&gt;
@@ -3335,9 +3383,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="EligibilityExpirationDate" type="xs:date" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The Eligibility Expiration Date is used to determine end of eligibility and to account for a child’s eligibility expiring earlier than 36 months from the child’s QAD. A child’s eligibility would end earlier than 36 months from the child’s
-              QAD, if the child is no longer entitled to a free public education (e.g., graduated with a high school diploma, obtained a high school equivalency diploma (HSED), or for other reasons as determined by States’ requirements), or if the child
-              passes away.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The Eligibility Expiration Date is used to determine end of eligibility and to account for a child’s eligibility expiring earlier than 36 months from the child’s QAD. A child’s eligibility would end earlier than 36 months from the child’s QAD, if the child is no longer entitled to a free public education (e.g., graduated with a high school diploma, obtained a high school equivalency diploma (HSED), or for other reasons as determined by States’ requirements), or if the child passes away.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="MigrantEducationProgramService" type="MigrantEducationProgramService" minOccurs="0" maxOccurs="unbounded"&gt;
@@ -3761,9 +3807,11 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="MedicallyFragile" type="xs:boolean" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Indicates whether the Student receiving special education and related services is: 1) in the age range of birth to 22 years, and 2) has a serious, ongoing illness or a chronic condition that has lasted or is anticipated to last at least 12
-              or more months or has required at least one month of hospitalization, and that requires daily, ongoing medical treatments and monitoring by appropriately trained personnel which may include parents or other family members, and 3) requires
-              the routine use of medical device or of assistive technology to compensate for the loss of usefulness of a body function needed to participate in activities of daily living, and 4) lives with ongoing threat to his or her continued well-being.
+            &lt;xs:documentation&gt;Indicates whether the Student receiving special education and related services is:
+              1) in the age range of birth to 22 years, and
+              2) has a serious, ongoing illness or a chronic condition that has lasted or is anticipated to last at least 12 or more months or has required at least one month of hospitalization, and that requires daily, ongoing medical treatments and monitoring by appropriately trained personnel which may include parents or other family members, and
+              3) requires the routine use of medical device or of assistive technology to compensate for the loss of usefulness of a body function needed to participate in activities of daily living, and
+              4) lives with ongoing threat to his or her continued well-being.
               Aligns with federal requirements.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
@@ -3944,8 +3992,11 @@
       &lt;xs:sequence&gt;
         &lt;xs:element name="TitleIPartAParticipant" type="TitleIPartAParticipantDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;An indication of the type of Title I program, if any, in which the student is participating and by which the student is served: Public Targeted Assistance Program Public Schoolwide Program Private School Students Participating Local Neglected
-              Program.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;An indication of the type of Title I program, if any, in which the student is participating and by which the student is served:
+              Public Targeted Assistance Program
+              Public Schoolwide Program
+              Private School Students Participating
+              Local Neglected Program.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;TitleIPartAParticipantDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -6388,13 +6439,13 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="NameOfCounty" type="NameOfCounty" minOccurs="0"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The name of the county, parish, borough, or comparable unit (within a state) in 'which an address is located.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The name of the county, parish, borough, or comparable unit (within a state) in
+          'which an address is located.&lt;/xs:documentation&gt;
       &lt;/xs:annotation&gt;
     &lt;/xs:element&gt;
     &lt;xs:element name="CountyFIPSCode" type="CountyFIPSCode" minOccurs="0"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The Federal Information Processing Standards (FIPS) numeric code for the county issued by the National Institute of Standards and Technology (NIST). Counties are considered to be the "first-order subdivisions" of each State and statistically equivalent
-          entity, regardless of their local designations (county, parish, borough, etc.) Counties in different States will have the same code. A unique county number is created when combined with the 2-digit FIPS State Code.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The Federal Information Processing Standards (FIPS) numeric code for the county issued by the National Institute of Standards and Technology (NIST). Counties are considered to be the "first-order subdivisions" of each State and statistically equivalent entity, regardless of their local designations (county, parish, borough, etc.) Counties in different States will have the same code. A unique county number is created when combined with the 2-digit FIPS State Code.&lt;/xs:documentation&gt;
       &lt;/xs:annotation&gt;
     &lt;/xs:element&gt;
     &lt;xs:element name="Latitude" type="Coordinate" minOccurs="0"&gt;
@@ -6530,8 +6581,10 @@
       <c r="H97" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="AssessmentPerformanceLevel"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;Definition of the performance levels and the associated cut scores. Three styles are supported: 1. Specification of performance level by minimum and maximum score 2. Specification of performance level by cut score, using only minimum score 3. Specification
-      of performance level without any mapping to scores&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;Definition of the performance levels and the associated cut scores. Three styles are supported:
+      1. Specification of performance level by minimum and maximum score
+      2. Specification of performance level by cut score, using only minimum score
+      3. Specification of performance level without any mapping to scores&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Common&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -6547,8 +6600,7 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="AssessmentReportingMethod" type="AssessmentReportingMethodDescriptorReferenceType"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The method that the instructor of the class uses to report the performance and achievement of all students. It may be a qualitative method such as individualized teacher comments or a quantitative method such as a letter or numerical grade. In
-          some cases, more than one type of reporting method may be used.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The method that the instructor of the class uses to report the performance and achievement of all students. It may be a qualitative method such as individualized teacher comments or a quantitative method such as a letter or numerical grade. In some cases, more than one type of reporting method may be used.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;AssessmentReportingMethodDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -6682,8 +6734,7 @@
   &lt;xs:sequence&gt;
     &lt;xs:element name="AssessmentReportingMethod" type="AssessmentReportingMethodDescriptorReferenceType"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The method that the administrator of the assessment uses to report the performance and achievement of all students. It may be a qualitative method such as performance level descriptors or a quantitative method such as a numerical grade or cut
-          score. More than one type of reporting method may be used.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The method that the administrator of the assessment uses to report the performance and achievement of all students. It may be a qualitative method such as performance level descriptors or a quantitative method such as a numerical grade or cut score. More than one type of reporting method may be used.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;AssessmentReportingMethodDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -6931,8 +6982,8 @@
       <c r="H103" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="ContentStandard"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;An indication as to whether an assessment conforms to a standard (e.g., local standard, statewide standard, regional standard, association standard). ...
-    &lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;An indication as to whether an assessment conforms to a standard (e.g., local standard, statewide standard, regional standard, association standard).
+      ...&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Common&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -7038,8 +7089,7 @@
   &lt;xs:sequence&gt;
     &lt;xs:element name="IdentificationCode" type="IdentificationCode"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;A unique number or alphanumeric code assigned to a course by a school, school system, state, or other agency or entity. For multi-part course codes, concatenate the parts separated by a "/". For example, consider the following SCED code- subject
-          = 20 Math course = 272 Geometry level = G General credits = 1.00 course sequence 1 of 1- would be entered as 20/272/G/1.00/1 of 1.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;A unique number or alphanumeric code assigned to a course by a school, school system, state, or other agency or entity. For multi-part course codes, concatenate the parts separated by a "/". For example, consider the following SCED code- subject = 20 Math course = 272 Geometry level = G General credits = 1.00 course sequence 1 of 1- would be entered as 20/272/G/1.00/1 of 1.&lt;/xs:documentation&gt;
       &lt;/xs:annotation&gt;
     &lt;/xs:element&gt;
     &lt;xs:element name="CourseIdentificationSystem" type="CourseIdentificationSystemDescriptorReferenceType"&gt;
@@ -7304,7 +7354,10 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="DiplomaLevel" type="DiplomaLevelDescriptorReferenceType" minOccurs="0"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The level of diploma/credential that is awarded to a student in recognition of his/her completion of the curricular requirements. Minimum high school program Recommended high school program Distinguished Achievement Program.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The level of diploma/credential that is awarded to a student in recognition of his/her completion of the curricular requirements.
+          Minimum high school program
+          Recommended high school program
+          Distinguished Achievement Program.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;DiplomaLevelDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -8022,8 +8075,7 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="InterventionEffectivenessRating" type="InterventionEffectivenessRatingDescriptorReferenceType"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;An intervention demonstrates effectiveness if the research has shown that the program caused an improvement in outcomes. Values: positive effects, potentially positive effects, mixed effects, potentially negative effects, negative effects, and
-          no discernible effects.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;An intervention demonstrates effectiveness if the research has shown that the program caused an improvement in outcomes. Values: positive effects, potentially positive effects, mixed effects, potentially negative effects, negative effects, and no discernible effects.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;InterventionEffectivenessRatingDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -8357,8 +8409,7 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="SchoolImprovementReservedFundsPercentage" type="Percent" minOccurs="0"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;An indication of the percentage of the Title I, Part A allocation that the SEA reserved in accordance with Section 1003(a) of ESEA and §200.100(a) of ED's regulations governing the reservation of funds for school improvement under Section 1003(a)
-          of ESEA.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;An indication of the percentage of the Title I, Part A allocation that the SEA reserved in accordance with Section 1003(a) of ESEA and §200.100(a) of ED's regulations governing the reservation of funds for school improvement under Section 1003(a) of ESEA.&lt;/xs:documentation&gt;
       &lt;/xs:annotation&gt;
     &lt;/xs:element&gt;
     &lt;xs:element name="SupplementalEducationalServicesFundsSpent" type="Currency" minOccurs="0"&gt;
@@ -8707,8 +8758,7 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="AssessmentReportingMethod" type="AssessmentReportingMethodDescriptorReferenceType"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The method that the instructor of the class uses to report the performance and achievement. It may be a qualitative method such as individualized teacher comments or a quantitative method such as a letter or numerical grade. In some cases, more
-          than one type of reporting method may be used.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The method that the instructor of the class uses to report the performance and achievement. It may be a qualitative method such as individualized teacher comments or a quantitative method such as a letter or numerical grade. In some cases, more than one type of reporting method may be used.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;AssessmentReportingMethodDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -9103,8 +9153,7 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="AssessmentReportingMethod" type="AssessmentReportingMethodDescriptorReferenceType"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The method that the administrator of the assessment uses to report the performance and achievement of all students. It may be a qualitative method such as performance level descriptors or a quantitative method such as a numerical grade or cut
-          score. More than one type of reporting method may be used.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The method that the administrator of the assessment uses to report the performance and achievement of all students. It may be a qualitative method such as performance level descriptors or a quantitative method such as a numerical grade or cut score. More than one type of reporting method may be used.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;AssessmentReportingMethodDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -9463,8 +9512,7 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="FederalProgramsFundingAllocation" type="Currency" minOccurs="0"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The amount of federal dollars distributed to Local Education Agencies (LEAs), retained by the State Education Agency (SEA) for program administration or other approved state-level activities (including unallocated, transferred to another state
-          agency, or distributed to entities other than LEAs).&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The amount of federal dollars distributed to Local Education Agencies (LEAs), retained by the State Education Agency (SEA) for program administration or other approved state-level activities (including unallocated, transferred to another state agency, or distributed to entities other than LEAs).&lt;/xs:documentation&gt;
       &lt;/xs:annotation&gt;
     &lt;/xs:element&gt;
   &lt;/xs:sequence&gt;
@@ -9526,8 +9574,12 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="ResponseIndicator" type="ResponseIndicatorDescriptorReferenceType" minOccurs="0"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;Indicator of the response. For example: Nonscorable response Ineffective response Effective response Partial response ...
-        &lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;Indicator of the response. For example:
+          Nonscorable response
+          Ineffective response
+          Effective response
+          Partial response
+          ...&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;ResponseIndicatorDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -9535,8 +9587,11 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="AssessmentItemResult" type="AssessmentItemResultDescriptorReferenceType"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;The analyzed result of a student's response to an assessment item. For example: Correct Incorrect Met standard ...
-        &lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;The analyzed result of a student's response to an assessment item. For example:
+          Correct
+          Incorrect
+          Met standard
+          ...&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;AssessmentItemResultDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -14791,8 +14846,11 @@
       <c r="H280" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="AdministrationEnvironmentDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;The environment in which the test was administered. For example: Electronic Classroom Testing Center ...
-    &lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;The environment in which the test was administered. For example:
+      Electronic
+      Classroom
+      Testing Center
+      ...&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -15017,8 +15075,11 @@
       <c r="H285" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="AssessmentItemResultDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;The analyzed result of a student's response to an assessment item.. For example: Correct Incorrect Met standard ...
-    &lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;The analyzed result of a student's response to an assessment item.. For example:
+      Correct
+      Incorrect
+      Met standard
+      ...&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -15110,8 +15171,7 @@
       <c r="H287" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="AssessmentReportingMethodDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This descriptor defines the method that the instructor of the class uses to report the performance and achievement of all students. It may be a qualitative method such as individualized teacher comments or a quantitative method such as a letter or
-      a numerical grade.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This descriptor defines the method that the instructor of the class uses to report the performance and achievement of all students. It may be a qualitative method such as individualized teacher comments or a quantitative method such as a letter or a numerical grade.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -15870,8 +15930,7 @@
       <c r="H304" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="ContinuationOfServicesReasonDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;In the Migrant Education program, a provision allows continuation of services after a child is no longer considered migratory for certain reasons. This descriptor holds the reasons prescribed in the statute. The mapping of descriptor values to known
-      Ed-Fi enumeration values is required.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;In the Migrant Education program, a provision allows continuation of services after a child is no longer considered migratory for certain reasons. This descriptor holds the reasons prescribed in the statute. The mapping of descriptor values to known Ed-Fi enumeration values is required.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -16009,8 +16068,11 @@
       <c r="H307" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="CourseAttemptResultDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;The result from the student's attempt to take the course, for example: Pass Fail Incomplete Withdrawn
-    &lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;The result from the student's attempt to take the course, for example:
+      Pass
+      Fail
+      Incomplete
+      Withdrawn&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -17953,8 +18015,7 @@
       <c r="H350" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="InterventionEffectivenessRatingDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;An intervention demonstrates effectiveness if the research has shown that the program caused an improvement in outcomes. Rating Values: positive effects, potentially positive effects, mixed effects, potentially negative effects, negative effects,
-      and no discernible effects.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;An intervention demonstrates effectiveness if the research has shown that the program caused an improvement in outcomes. Rating Values: positive effects, potentially positive effects, mixed effects, potentially negative effects, negative effects, and no discernible effects.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -18317,8 +18378,7 @@
       <c r="H358" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="LimitedEnglishProficiencyDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This descriptor defines the indications that the student has been identified as limited English proficient by the Language Proficiency Assessment Committee (LPAC), or English proficient. The mapping of descriptor values to known Ed-Fi enumeration
-      values is required.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This descriptor defines the indications that the student has been identified as limited English proficient by the Language Proficiency Assessment Committee (LPAC), or English proficient. The mapping of descriptor values to known Ed-Fi enumeration values is required.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -18406,8 +18466,7 @@
       <c r="H360" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="MagnetSpecialProgramEmphasisSchoolDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;A school that has been designed to attract students of different racial/ethnic backgrounds for the purpose of reducing, preventing or eliminating racial isolation; and/or to provide an academic or social focus on a particular theme (e.g., science/math,
-      performing arts, gifted/talented, or foreign language).&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;A school that has been designed to attract students of different racial/ethnic backgrounds for the purpose of reducing, preventing or eliminating racial isolation; and/or to provide an academic or social focus on a particular theme (e.g., science/math, performing arts, gifted/talented, or foreign language).&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -19843,8 +19902,15 @@
       <c r="H392" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="ReasonNotTestedDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;The primary reason student is not tested. For example: Absent Refusal by parent Refusal by student Medical waiver Illness Disruptive behavior LEP Exempt '...
-    &lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;The primary reason student is not tested. For example:
+      Absent
+      Refusal by parent
+      Refusal by student
+      Medical waiver
+      Illness
+      Disruptive behavior
+      LEP Exempt
+      '...&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -20113,8 +20179,12 @@
       <c r="H398" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="ResponseIndicatorDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;Indicator of the response. For example: Nonscorable response Ineffective response Effective response Partial response ...
-    &lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;Indicator of the response. For example:
+      Nonscorable response
+      Ineffective response
+      Effective response
+      Partial response
+      ...&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -20297,8 +20367,11 @@
       <c r="H402" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="RetestIndicatorDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;Indicator if the test was retaken. For example: Primary administration First retest Second retest ...
-    &lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;Indicator if the test was retaken. For example:
+      Primary administration
+      First retest
+      Second retest
+      ...&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -21353,16 +21426,16 @@
     </row>
     <row r="426" xml:space="preserve">
       <c r="A426" t="str">
-        <v>596</v>
+        <v>247</v>
       </c>
       <c r="B426" t="str">
-        <v>EducationOrganizationNetworkAssociation</v>
+        <v>TitleIPartAParticipant</v>
       </c>
       <c r="C426" t="str">
-        <v>Properties of the association between the EducationOrganization and its network(s).</v>
+        <v>An indication of the type of Title I program, if any, in which the student is participating and served.</v>
       </c>
       <c r="D426" t="str">
-        <v>Association</v>
+        <v>Descriptor</v>
       </c>
       <c r="E426" t="str">
         <v/>
@@ -21371,60 +21444,27 @@
         <v/>
       </c>
       <c r="G426" t="str" xml:space="preserve">
-        <v xml:space="preserve">Contains:
-BeginDate (optional)
-EducationOrganization (identity)
-EducationOrganizationNetwork (identity)
-EndDate (optional)</v>
+        <v xml:space="preserve">Used By:
+StudentTitleIPartAProgramAssociation.TitleIPartAParticipant (as required)</v>
       </c>
       <c r="H426" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;xs:complexType name="EducationOrganizationNetworkAssociation"&gt;
-  &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;Properties of the association between the EducationOrganization and its network(s).&lt;/xs:documentation&gt;
-    &lt;xs:appinfo&gt;
-      &lt;ann:TypeGroup&gt;Association&lt;/ann:TypeGroup&gt;
+        <v xml:space="preserve">&lt;xs:complexType name="TitleIPartAParticipantDescriptor"&gt;
+  &lt;xs:annotation&gt;
+    &lt;xs:documentation&gt;An indication of the type of Title I program, if any, in which the student is participating and served.&lt;/xs:documentation&gt;
+    &lt;xs:appinfo&gt;
+      &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
   &lt;/xs:annotation&gt;
   &lt;xs:complexContent&gt;
-    &lt;xs:extension base="ComplexObjectType"&gt;
-      &lt;xs:sequence&gt;
-        &lt;xs:element name="EducationOrganizationNetworkReference" type="EducationOrganizationNetworkReferenceType"&gt;
-          &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;A reference to the EducationOrganizationNetwork to which this education organization is a member.&lt;/xs:documentation&gt;
-          &lt;/xs:annotation&gt;
-        &lt;/xs:element&gt;
-        &lt;xs:element name="MemberEducationOrganizationReference" type="EducationOrganizationReferenceType"&gt;
-          &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The EducationOrganization member in the network.&lt;/xs:documentation&gt;
-          &lt;/xs:annotation&gt;
-        &lt;/xs:element&gt;
-        &lt;xs:element name="BeginDate" type="xs:date" minOccurs="0"&gt;
-          &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The date on which the EducationOrganization joined this network.&lt;/xs:documentation&gt;
-          &lt;/xs:annotation&gt;
-        &lt;/xs:element&gt;
-        &lt;xs:element name="EndDate" type="xs:date" minOccurs="0"&gt;
-          &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The date on which the EducationOrganization left this network.&lt;/xs:documentation&gt;
-          &lt;/xs:annotation&gt;
-        &lt;/xs:element&gt;
-      &lt;/xs:sequence&gt;
-    &lt;/xs:extension&gt;
+    &lt;xs:extension base="DescriptorType" /&gt;
   &lt;/xs:complexContent&gt;
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I426" t="str" xml:space="preserve">
-        <v xml:space="preserve">edfi.EducationOrganizationNetworkAssociation
-EducationOrganizationNetworkId [INT] NOT NULL
-MemberEducationOrganizationId [INT] NOT NULL
-BeginDate [DATE] NULL
-EndDate [DATE] NULL
-CreateDate [DATETIME] NOT NULL
-LastModifiedDate [DATETIME] NOT NULL
-Id [UNIQUEIDENTIFIER] NOT NULL
-Primary Keys:
-EducationOrganizationNetworkId
-MemberEducationOrganizationId
+        <v xml:space="preserve">edfi.TitleIPartAParticipantDescriptor
+TitleIPartAParticipantDescriptorId [INT] NOT NULL
+Primary Keys:
+TitleIPartAParticipantDescriptorId
 </v>
       </c>
     </row>
@@ -22106,8 +22146,7 @@
       <c r="H436" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="Assessment"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This entity represents a tool, instrument, process, or exhibition composed of a systematic sampling of behavior for measuring a student's competence, knowledge, skills, or behavior. An assessment can be used to measure differences in individuals or
-      groups and changes in performance from one occasion to the next.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This entity represents a tool, instrument, process, or exhibition composed of a systematic sampling of behavior for measuring a student's competence, knowledge, skills, or behavior. An assessment can be used to measure differences in individuals or groups and changes in performance from one occasion to the next.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -22127,8 +22166,13 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="AssessmentCategory" type="AssessmentCategoryDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The category of an assessment based on format and content. For example: Achievement test Advanced placement test Alternate assessment/grade-level standards Attitudinal test Cognitive and perceptual skills test ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The category of an assessment based on format and content. For example:
+              Achievement test
+              Advanced placement test
+              Alternate assessment/grade-level standards
+              Attitudinal test
+              Cognitive and perceptual skills test
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;AssessmentCategoryDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -22145,8 +22189,11 @@
         &lt;xs:element name="AssessedGradeLevel" type="GradeLevelDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
             &lt;xs:documentation&gt;The typical grade level for which an assessment is designed. If the assessment spans a range of grades, then this attribute holds the highest grade assessed. If only one grade level is assessed then only this attribute is used. For example:
-              Adult Prekindergarten First grade Second grade ...
-            &lt;/xs:documentation&gt;
+              Adult
+              Prekindergarten
+              First grade
+              Second grade
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;GradeLevelDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -22154,8 +22201,12 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="LowestAssessedGradeLevel" type="GradeLevelDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;If the assessment spans a range of grades, then this attribute holds the lowest grade assessed. If only one grade level is assessed, then this attribute is omitted. For example: Adult Prekindergarten First grade Second grade ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;If the assessment spans a range of grades, then this attribute holds the lowest grade assessed. If only one grade level is assessed, then this attribute is omitted. For example:
+              Adult
+              Prekindergarten
+              First grade
+              Second grade
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;GradeLevelDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -22168,7 +22219,9 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="AssessmentPerformanceLevel" type="AssessmentPerformanceLevel" minOccurs="0" maxOccurs="unbounded"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Definition of the performance levels and the associated cut scores. Three styles are supported: 1. Specification of performance level by minimum and maximum score 2. Specification of performance level by cut score, using only minimum score
+            &lt;xs:documentation&gt;Definition of the performance levels and the associated cut scores. Three styles are supported:
+              1. Specification of performance level by minimum and maximum score
+              2. Specification of performance level by cut score, using only minimum score
               3. Specification of performance level without any mapping to scores.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
@@ -22466,8 +22519,11 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="AssessmentItemCategory" type="AssessmentItemCategoryDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Category or type of the AssessmentItem. For example: Multiple choice Analytic Prose ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Category or type of the AssessmentItem. For example:
+              Multiple choice
+              Analytic
+              Prose
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;AssessmentItemCategoryDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -23298,8 +23354,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="SuccessCriteria" type="Criteria" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;One or more statements that describes the criteria used by teachers and students to check for attainment of a competency objective. This criteria gives clear indications as to the degree to which learning is moving through the Zone or Proximal
-              Development toward independent achievement of the CompetencyObjective.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;One or more statements that describes the criteria used by teachers and students to check for attainment of a competency objective. This criteria gives clear indications as to the degree to which learning is moving through the Zone or Proximal Development toward independent achievement of the CompetencyObjective.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
       &lt;/xs:sequence&gt;
@@ -23354,8 +23409,7 @@
       <c r="H446" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="ContractedStaff"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This financial entity represents the sum of the financial transactions to date for contracted staff. ContractedStaff includes "contractors" or "consultants" who perform services for an agreed upon fee, or an employee of a management service contracted
-      to work on site.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This financial entity represents the sum of the financial transactions to date for contracted staff. ContractedStaff includes "contractors" or "consultants" who perform services for an agreed upon fee, or an employee of a management service contracted to work on site.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -23473,9 +23527,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="CourseTitle" type="CourseTitle"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The descriptive name given to a course of study offered in a school or other institution or organization. In departmentalized classes at the elementary, secondary, and postsecondary levels (and for staff development activities), this refers
-              to the name by which a course is identified (e.g., American History, English III). For elementary and other non-departmentalized classes, it refers to any portion of the instruction for which a grade or report is assigned (e.g., reading,
-              composition, spelling, and language arts).&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The descriptive name given to a course of study offered in a school or other institution or organization. In departmentalized classes at the elementary, secondary, and postsecondary levels (and for staff development activities), this refers to the name by which a course is identified (e.g., American History, English III). For elementary and other non-departmentalized classes, it refers to any portion of the instruction for which a grade or report is assigned (e.g., reading, composition, spelling, and language arts).&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="NumberOfParts" type="NumberOfParts"&gt;
@@ -23858,8 +23910,11 @@
       &lt;xs:sequence&gt;
         &lt;xs:element name="CourseAttemptResult" type="CourseAttemptResultDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The result from the student's attempt to take the course, for example: Pass Fail Incomplete Withdrawn.
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The result from the student's attempt to take the course, for example:
+              Pass
+              Fail
+              Incomplete
+              Withdrawn.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;CourseAttemptResultDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -23926,9 +23981,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="CourseTitle" type="CourseTitle" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The descriptive name given to a course of study offered in a school or other institution or organization. In departmentalized classes at the elementary, secondary, and postsecondary levels (and for staff development activities), this refers
-              to the name by which a course is identified (e.g., American History, English III). For elementary and other non-departmentalized classes, it refers to any portion of the instruction for which a grade or report is assigned (e.g., reading,
-              composition, spelling, language arts).&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The descriptive name given to a course of study offered in a school or other institution or organization. In departmentalized classes at the elementary, secondary, and postsecondary levels (and for staff development activities), this refers to the name by which a course is identified (e.g., American History, English III). For elementary and other non-departmentalized classes, it refers to any portion of the instruction for which a grade or report is assigned (e.g., reading, composition, spelling, language arts).&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="AlternativeCourseTitle" type="CourseTitle" minOccurs="0"&gt;
@@ -24427,8 +24480,7 @@
       <c r="H452" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="DisciplineIncident"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This event entity represents an occurrence of an infraction ranging from a minor behavioral problem that disrupts the orderly functioning of a school or classroom (such as tardiness) to a criminal act that results in the involvement of a law enforcement
-      official (such as robbery). A single event (e.g., a fight) is one incident regardless of how many perpetrators or victims are involved. Discipline incidents are events classified as warranting discipline action.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This event entity represents an occurrence of an infraction ranging from a minor behavioral problem that disrupts the orderly functioning of a school or classroom (such as tardiness) to a criminal act that results in the involvement of a law enforcement official (such as robbery). A single event (e.g., a fight) is one incident regardless of how many perpetrators or victims are involved. Discipline incidents are events classified as warranting discipline action.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -24438,8 +24490,7 @@
       &lt;xs:sequence&gt;
         &lt;xs:element name="IncidentIdentifier" type="IncidentIdentifier"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;A locally assigned unique identifier (within the school or school district) to identify each specific DisciplineIncident or occurrence. The same identifier should be used to document the entire DisciplineIncident even if it included multiple
-              offenses and multiple offenders.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;A locally assigned unique identifier (within the school or school district) to identify each specific DisciplineIncident or occurrence. The same identifier should be used to document the entire DisciplineIncident even if it included multiple offenses and multiple offenders.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="IncidentDate" type="xs:date"&gt;
@@ -24454,8 +24505,13 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="IncidentLocation" type="IncidentLocationDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Identifies where the DisciplineIncident occurred and whether or not it occurred on school, for example: On school Administrative offices area Cafeteria area Classroom Hallway or stairs ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Identifies where the DisciplineIncident occurred and whether or not it occurred on school, for example:
+              On school
+              Administrative offices area
+              Cafeteria area
+              Classroom
+              Hallway or stairs
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;IncidentLocationDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -24468,9 +24524,13 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="ReporterDescription" type="ReporterDescriptionDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Information on the type of individual who reported the DisciplineIncident. When known and/or if useful, use a more specific option code (e.g., "Counselor" rather than "Professional Staff"); for example: Student Parent/guardian Law enforcement
-              officer Nonschool personnel Representative of visiting school ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Information on the type of individual who reported the DisciplineIncident. When known and/or if useful, use a more specific option code (e.g., "Counselor" rather than "Professional Staff"); for example:
+              Student
+              Parent/guardian
+              Law enforcement officer
+              Nonschool personnel
+              Representative of visiting school
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;ReporterDescriptionDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -24506,8 +24566,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="IncidentCost" type="Currency" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The value of any quantifiable monetary loss directly resulting from the DisciplineIncident. Examples include the value of repairs necessitated by vandalism of a school facility, or the value of personnel resources used for repairs or consumed
-              by the incident.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The value of any quantifiable monetary loss directly resulting from the DisciplineIncident. Examples include the value of repairs necessitated by vandalism of a school facility, or the value of personnel resources used for repairs or consumed by the incident.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="SchoolReference" type="SchoolReferenceType"&gt;
@@ -24599,8 +24658,7 @@
       <c r="H453" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="EducationContent"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This entity represents materials for students or teachers that can be used for teaching, learning, research, and more. Education content includes full courses, course materials, modules, intervention descriptions, textbooks, streaming videos, tests,
-      software, and any other tools, materials, or techniques used to support access to knowledge.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This entity represents materials for students or teachers that can be used for teaching, learning, research, and more. Education content includes full courses, course materials, modules, intervention descriptions, textbooks, streaming videos, tests, software, and any other tools, materials, or techniques used to support access to knowledge.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -25363,8 +25421,7 @@
       <c r="H458" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="GraduationPlan"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This entity is a plan outlining the required credits, credits by subject, credits by course, and other criteria required for graduation. A graduation plan may be one or more standard plans defined by an education organization and/or individual plans
-      for some or all students.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This entity is a plan outlining the required credits, credits by subject, credits by course, and other criteria required for graduation. A graduation plan may be one or more standard plans defined by an education organization and/or individual plans for some or all students.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -25862,8 +25919,7 @@
       &lt;xs:sequence&gt;
         &lt;xs:element name="EducationContentSource" type="EducationContentSource"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Resources related to or used in this intervention prescription, including any documentation around the InterventionPrescription itself. Since an intervention prescription is intended to be a published intervention, an intervention prescription
-              should have at least one such resource.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Resources related to or used in this intervention prescription, including any documentation around the InterventionPrescription itself. Since an intervention prescription is intended to be a published intervention, an intervention prescription should have at least one such resource.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="InterventionClass" type="InterventionClassDescriptorReferenceType"&gt;
@@ -26337,8 +26393,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="SuccessCriteria" type="Criteria" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;One or more statements that describes the criteria used by teachers and students to check for attainment of a learning objective. This criteria gives clear indications as to the degree to which learning is moving through the Zone or Proximal
-              Development toward independent achievement of the LearningObjective.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;One or more statements that describes the criteria used by teachers and students to check for attainment of a learning objective. This criteria gives clear indications as to the degree to which learning is moving through the Zone or Proximal Development toward independent achievement of the LearningObjective.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="LearningStandardReference" type="LearningStandardReferenceType" minOccurs="0" maxOccurs="unbounded"&gt;
@@ -26493,8 +26548,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="Description" type="Description"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The text of the statement. The textual content that either describes a specific competency such as "Apply the Pythagorean Theorem to determine unknown side lengths in right triangles in real-world and mathematical problems in two and three
-              dimensions." or describes a less granular group of competencies within the taxonomy of the standards document, e.g. "Understand and apply the Pythagorean Theorem," or "Geometry".&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The text of the statement. The textual content that either describes a specific competency such as "Apply the Pythagorean Theorem to determine unknown side lengths in right triangles in real-world and mathematical problems in two and three dimensions." or describes a less granular group of competencies within the taxonomy of the standards document, e.g. "Understand and apply the Pythagorean Theorem," or "Geometry".&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="LearningStandardItemCode" type="IdentificationCode" minOccurs="0"&gt;
@@ -26535,14 +26589,12 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="SuccessCriteria" type="Criteria" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;One or more statements that describes the criteria used by teachers and students to check for attainment of a learning standard. This criteria gives clear indications as to the degree to which learning is moving through the Zone or Proximal
-              Development toward independent achievement of the LearningStandard.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;One or more statements that describes the criteria used by teachers and students to check for attainment of a learning standard. This criteria gives clear indications as to the degree to which learning is moving through the Zone or Proximal Development toward independent achievement of the LearningStandard.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="PrerequisiteLearningStandardReference" type="LearningStandardReferenceType" minOccurs="0" maxOccurs="unbounded"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The unique identifier of a prerequisite learning standard item, a competency needed prior to learning this one. (Some items may have no prerequisites others may have one or more prerequisites. This should only be used to represent the immediate
-              predecessors in a competency-based pathway, i.e. not prerequisites of prerequisites).&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The unique identifier of a prerequisite learning standard item, a competency needed prior to learning this one. (Some items may have no prerequisites others may have one or more prerequisites. This should only be used to represent the immediate predecessors in a competency-based pathway, i.e. not prerequisites of prerequisites).&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="ParentLearningStandardReference" type="LearningStandardReferenceType" minOccurs="0"&gt;
@@ -26771,7 +26823,9 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="AssessmentPerformanceLevel" type="AssessmentPerformanceLevel" minOccurs="0" maxOccurs="unbounded"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Definition of the performance levels and the associated cut scores. Three styles are supported: 1. Specification of performance level by minimum and maximum score 2. Specification of performance level by cut score, using only minimum score
+            &lt;xs:documentation&gt;Definition of the performance levels and the associated cut scores. Three styles are supported:
+              1. Specification of performance level by minimum and maximum score
+              2. Specification of performance level by cut score, using only minimum score
               3. Specification of performance level without any mapping to scores.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
@@ -26978,8 +27032,13 @@
       &lt;xs:sequence&gt;
         &lt;xs:element name="EmploymentStatus" type="EmploymentStatusDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Reflects the type of employment or contract desired for the position; for example: Probationary Contractual Substitute/temporary Tenured or permanent Volunteer/no contract ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Reflects the type of employment or contract desired for the position; for example:
+              Probationary
+              Contractual
+              Substitute/temporary
+              Tenured or permanent
+              Volunteer/no contract
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;EmploymentStatusDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -27005,7 +27064,12 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="ProgramAssignment" type="ProgramAssignmentDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The name of the program for which the OpenStaffPosition will be assigned; for example: Regular education Title I-Academic Title I-Non-Academic Special Education' Bilingual/English as a Second Language.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The name of the program for which the OpenStaffPosition will be assigned; for example:
+              Regular education
+              Title I-Academic
+              Title I-Non-Academic
+              Special Education'
+              Bilingual/English as a Second Language.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;ProgramAssignmentDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -27352,8 +27416,7 @@
       <c r="H468" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="Payroll"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This financial entity represents the sum of the financial transactions to date for employee compensation. An "employee" who performs services under the direction of the employing institution or agency, is compensated for such services by the employer
-      and is eligible for employee benefits and wage or salary tax withholdings.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This financial entity represents the sum of the financial transactions to date for employee compensation. An "employee" who performs services under the direction of the employing institution or agency, is compensated for such services by the employer and is eligible for employee benefits and wage or salary tax withholdings.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -27529,8 +27592,7 @@
       <c r="H470" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="Program"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This entity represents any program designed to work in conjunction with, or as a supplement to, the main academic program. Programs may provide instruction, training, services, or benefits through federal, state, or local agencies. Programs may also
-      include organized extracurricular activities for students.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This entity represents any program designed to work in conjunction with, or as a supplement to, the main academic program. Programs may provide instruction, training, services, or benefits through federal, state, or local agencies. Programs may also include organized extracurricular activities for students.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -27910,8 +27972,7 @@
       <c r="H472" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="RestraintEvent"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This event entity represents the instances where a special education student was physically or mechanically restrained due to imminent serious physical harm to themselves or others, imminent serious property destruction or a combination of both imminent
-      serious physical harm to themselves or others and imminent serious property destruction.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This event entity represents the instances where a special education student was physically or mechanically restrained due to imminent serious physical harm to themselves or others, imminent serious property destruction or a combination of both imminent serious physical harm to themselves or others and imminent serious property destruction.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -28074,8 +28135,13 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="EducationalEnvironment" type="EducationalEnvironmentDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The setting in which a child receives education and related services; for example: Center-based instruction Home-based instruction Hospital class Mainstream Residential care and treatment facility ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The setting in which a child receives education and related services; for example:
+              Center-based instruction
+              Home-based instruction
+              Hospital class
+              Mainstream
+              Residential care and treatment facility
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;EducationalEnvironmentDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -28083,9 +28149,13 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="MediumOfInstruction" type="MediumOfInstructionDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The media through which teachers provide instruction to students and students and teachers communicate about instructional matters; for example: Technology-based instruction in classroom Correspondence instruction Face-to-face instruction
-              Virtual/On-line Distance learning Center-based instruction ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The media through which teachers provide instruction to students and students and teachers communicate about instructional matters; for example:
+              Technology-based instruction in classroom
+              Correspondence instruction
+              Face-to-face instruction
+              Virtual/On-line Distance learning
+              Center-based instruction
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;MediumOfInstructionDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -28093,8 +28163,13 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="PopulationServed" type="PopulationServedDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The type of students the Section is offered and tailored to; for example: Bilingual students Remedial education students Gifted and talented students Career and Technical Education students Special education students ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The type of students the Section is offered and tailored to; for example:
+              Bilingual students
+              Remedial education students
+              Gifted and talented students
+              Career and Technical Education students
+              Special education students
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;PopulationServedDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -28102,8 +28177,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="AvailableCredits" type="Credits" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The amount of credit available to a student who successfully meets the objectives of the course. AvailableCredits are measured in Carnegie units, A course meeting every day for one period of the school day over the span of a school year offers
-              one Carnegie unit. See publication: U.S. Department of Education, NCES, 2007-341, Secondary School Course Classification System: School Codes for the Exchange of Data (SCED).&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The amount of credit available to a student who successfully meets the objectives of the course. AvailableCredits are measured in Carnegie units, A course meeting every day for one period of the school day over the span of a school year offers one Carnegie unit. See publication: U.S. Department of Education, NCES, 2007-341, Secondary School Course Classification System: School Codes for the Exchange of Data (SCED).&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="SectionCharacteristic" type="SectionCharacteristicDescriptorReferenceType" minOccurs="0" maxOccurs="unbounded"&gt;
@@ -28530,10 +28604,12 @@
       <c r="H476" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="Staff"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This entity represents an individual who performs specified activities for any public or private education institution or agency that provides instructional and/or support services to students or staff at the early childhood level through high school
-      completion. For example, this includes: 1. An "employee" who performs services under the direction of the employing institution or agency is compensated for such services by the employer and is eligible for employee benefits and wage or salary tax
-      withholdings 2. A "contractor" or "consultant" who performs services for an agreed upon fee or an employee of a management service contracted to work on site 3. A "volunteer" who performs services on a voluntary and uncompensated basis 4. An in-kind
-      service provider 5. An independent contractor or businessperson working at a school site.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This entity represents an individual who performs specified activities for any public or private education institution or agency that provides instructional and/or support services to students or staff at the early childhood level through high school completion. For example, this includes:
+      1. An "employee" who performs services under the direction of the employing institution or agency is compensated for such services by the employer and is eligible for employee benefits and wage or salary tax withholdings
+      2. A "contractor" or "consultant" who performs services for an agreed upon fee or an employee of a management service contracted to work on site
+      3. A "volunteer" who performs services on a voluntary and uncompensated basis
+      4. An in-kind service provider
+      5. An independent contractor or businessperson working at a school site.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -28596,13 +28672,17 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="HispanicLatinoEthnicity" type="xs:boolean" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;An indication that the individual traces his or her origin or descent to Mexico, Puerto Rico, Cuba, Central, and South America, and other Spanish cultures, regardless of race. The term, "Spanish origin," can be used in addition to "Hispanic
-              or Latino."&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;An indication that the individual traces his or her origin or descent to Mexico, Puerto Rico, Cuba, Central, and South America, and other Spanish cultures, regardless of race. The term, "Spanish origin," can be used in addition to "Hispanic or Latino."&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="OldEthnicity" type="OldEthnicityDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Previous definition of Ethnicity combining Hispanic/Latino and race: 1 - American Indian or Alaskan Native 2 - Asian or Pacific Islander 3 - Black, not of Hispanic origin 4 - Hispanic 5 - White, not of Hispanic origin.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Previous definition of Ethnicity combining Hispanic/Latino and race:
+              1 - American Indian or Alaskan Native
+              2 - Asian or Pacific Islander
+              3 - Black, not of Hispanic origin
+              4 - Hispanic
+              5 - White, not of Hispanic origin.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;OldEthnicityDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -28610,8 +28690,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="Race" type="RaceDescriptorReferenceType" minOccurs="0" maxOccurs="unbounded"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The general racial category which most clearly reflects the individual's recognition of his or her community or with which the individual most identifies. The way this data element is listed, it must allow for multiple entries so that each
-              individual can specify all appropriate races.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The general racial category which most clearly reflects the individual's recognition of his or her community or with which the individual most identifies. The way this data element is listed, it must allow for multiple entries so that each individual can specify all appropriate races.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;RaceDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -29024,8 +29103,10 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="StaffLeaveEventCategory" type="StaffLeaveEventCategoryDescriptorReferenceType"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The code describing the type of leave taken, for example: Sick Personal Vacation.
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The code describing the type of leave taken, for example:
+              Sick
+              Personal
+              Vacation.&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;StaffLeaveEventCategoryDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -29126,8 +29207,7 @@
       <c r="H479" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="Student"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This entity represents an individual for whom instruction, services, and/or care are provided in an early childhood, elementary, or secondary educational program under the jurisdiction of a school, education agency or other institution or program.
-      A student is a person who has been enrolled in a school or other educational institution.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This entity represents an individual for whom instruction, services, and/or care are provided in an early childhood, elementary, or secondary educational program under the jurisdiction of a school, education agency or other institution or program. A student is a person who has been enrolled in a school or other educational institution.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -29305,20 +29385,17 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="CumulativeGradePointsEarned" type="GPA" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The cumulative number of grade points an individual earns by successfully completing courses or examinations during his or her enrollment in the current school as well as those transferred from schools in which the individual had been previously
-              enrolled.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The cumulative number of grade points an individual earns by successfully completing courses or examinations during his or her enrollment in the current school as well as those transferred from schools in which the individual had been previously enrolled.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="CumulativeGradePointAverage" type="GPA" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;A measure of average performance in all courses taken by an individual during his or her school career as determined for record-keeping purposes. This is obtained by dividing the total grade points received by the total number of credits attempted.
-              This usually includes grade points received and credits attempted in his or her current school as well as those transferred from schools in which the individual was previously enrolled.&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;A measure of average performance in all courses taken by an individual during his or her school career as determined for record-keeping purposes. This is obtained by dividing the total grade points received by the total number of credits attempted. This usually includes grade points received and credits attempted in his or her current school as well as those transferred from schools in which the individual was previously enrolled.&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="GradeValueQualifier" type="GradeValueQualifier" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The scale of equivalents, if applicable, for grades awarded as indicators of performance in schoolwork. For example, numerical equivalents for letter grades used in determining a student's Grade Point Average (A=4, B=3, C=2, D=1 in a four-point
-              system) or letter equivalents for percentage grades (90-100%=A, 80-90%=B, etc.)&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The scale of equivalents, if applicable, for grades awarded as indicators of performance in schoolwork. For example, numerical equivalents for letter grades used in determining a student's Grade Point Average (A=4, B=3, C=2, D=1 in a four-point system) or letter equivalents for percentage grades (90-100%=A, 80-90%=B, etc.)&lt;/xs:documentation&gt;
           &lt;/xs:annotation&gt;
         &lt;/xs:element&gt;
         &lt;xs:element name="ClassRanking" type="ClassRanking" minOccurs="0"&gt;
@@ -29623,8 +29700,11 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="AdministrationEnvironment" type="AdministrationEnvironmentDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The environment in which the test was administered. For example: Electronic Classroom Testing Center ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The environment in which the test was administered. For example:
+              Electronic
+              Classroom
+              Testing Center
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;AdministrationEnvironmentDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -29632,9 +29712,14 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="Accommodation" type="AccommodationDescriptorReferenceType" minOccurs="0" maxOccurs="unbounded"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The specific type of special variation used in how an examination is presented, how it is administered, or how the test taker is allowed to respond. This generally refers to changes that do not substantially alter what the examination measures.
-              The proper use of accommodations does not substantially change academic level or performance criteria. For example: Braille Enlarged monitor view Extra time Large Print Setting Oral Administration ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The specific type of special variation used in how an examination is presented, how it is administered, or how the test taker is allowed to respond. This generally refers to changes that do not substantially alter what the examination measures. The proper use of accommodations does not substantially change academic level or performance criteria. For example:
+              Braille
+              Enlarged monitor view
+              Extra time
+              Large Print
+              Setting
+              Oral Administration
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;AccommodationDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -29642,8 +29727,11 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="RetestIndicator" type="RetestIndicatorDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;Indicator if the test was retaken. For example: Primary administration First retest Second retest ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;Indicator if the test was retaken. For example:
+              Primary administration
+              First retest
+              Second retest
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;RetestIndicatorDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -29651,8 +29739,15 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="ReasonNotTested" type="ReasonNotTestedDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;The primary reason student is not tested. For example: Absent Refusal by parent Refusal by student Medical waiver Illness Disruptive behavior LEP Exempt ...
-            &lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;The primary reason student is not tested. For example:
+              Absent
+              Refusal by parent
+              Refusal by student
+              Medical waiver
+              Illness
+              Disruptive behavior
+              LEP Exempt
+              ...&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;ReasonNotTestedDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -31016,8 +31111,7 @@
       <c r="H493" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="LocalEducationAgency"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;This entity represents an administrative unit at the local level which exists primarily to operate schools or to contract for educational services. It includes school districts, charter schools, charter management organizations, or other local administrative
-      organizations.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;This entity represents an administrative unit at the local level which exists primarily to operate schools or to contract for educational services. It includes school districts, charter schools, charter management organizations, or other local administrative organizations.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Domain Entity&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -31176,8 +31270,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="AdministrativeFundingControl" type="AdministrativeFundingControlDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;A classification of whether a postsecondary institution is operated by publicly elected or appointed officials (public control) or by privately elected or appointed officials and derives its major source of funds from private sources (private
-              control).&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;A classification of whether a postsecondary institution is operated by publicly elected or appointed officials (public control) or by privately elected or appointed officials and derives its major source of funds from private sources (private control).&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;AdministrativeFundingControlDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -31326,8 +31419,7 @@
         &lt;/xs:element&gt;
         &lt;xs:element name="MagnetSpecialProgramEmphasisSchool" type="MagnetSpecialProgramEmphasisSchoolDescriptorReferenceType" minOccurs="0"&gt;
           &lt;xs:annotation&gt;
-            &lt;xs:documentation&gt;A school that has been designed: 1) to attract students of different racial/ethnic backgrounds for the purpose of reducing, preventing, or eliminating racial isolation; and/or 2) to provide an academic or social focus on a particular theme
-              (e.g., science/math, performing arts, gifted/talented, or foreign language).&lt;/xs:documentation&gt;
+            &lt;xs:documentation&gt;A school that has been designed: 1) to attract students of different racial/ethnic backgrounds for the purpose of reducing, preventing, or eliminating racial isolation; and/or 2) to provide an academic or social focus on a particular theme (e.g., science/math, performing arts, gifted/talented, or foreign language).&lt;/xs:documentation&gt;
             &lt;xs:appinfo&gt;
               &lt;ann:Descriptor&gt;MagnetSpecialProgramEmphasisSchoolDescriptor&lt;/ann:Descriptor&gt;
             &lt;/xs:appinfo&gt;
@@ -31624,8 +31716,11 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="AttendanceEventCategory" type="AttendanceEventCategoryDescriptorReferenceType"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;A code describing the attendance event, for example: Present Unexcused absence Excused absence Tardy.
-        &lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;A code describing the attendance event, for example:
+          Present
+          Unexcused absence
+          Excused absence
+          Tardy.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;AttendanceEventCategoryDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -31975,7 +32070,9 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="Separation" type="SeparationDescriptorReferenceType" minOccurs="0"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;Type of employment separation; for example: Voluntary separation, Involuntary separation, Mutual agreement Other, etc.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;Type of employment separation; for example: Voluntary separation, Involuntary separation,
+          Mutual agreement
+          Other, etc.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;SeparationDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;
@@ -31983,7 +32080,12 @@
     &lt;/xs:element&gt;
     &lt;xs:element name="SeparationReason" type="SeparationReasonDescriptorReferenceType" minOccurs="0"&gt;
       &lt;xs:annotation&gt;
-        &lt;xs:documentation&gt;Reason for terminating the employment; for example: Employment in education Employment outside of education Retirement Family/personal relocation Change of assignment.&lt;/xs:documentation&gt;
+        &lt;xs:documentation&gt;Reason for terminating the employment; for example:
+          Employment in education
+          Employment outside of education
+          Retirement
+          Family/personal relocation
+          Change of assignment.&lt;/xs:documentation&gt;
         &lt;xs:appinfo&gt;
           &lt;ann:Descriptor&gt;SeparationReasonDescriptor&lt;/ann:Descriptor&gt;
         &lt;/xs:appinfo&gt;

</xml_diff>